<commit_message>
added pages controller and views, and connected them with router
</commit_message>
<xml_diff>
--- a/resources/API docs.xlsx
+++ b/resources/API docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arturaronov/Desktop/Programming/fswdi/unit-2/unit-2-project/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72979C35-00D0-9944-BAEF-2EA9A522DBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE2AFD6-C572-434B-8F1C-10E5F13079FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10100" yWindow="500" windowWidth="23500" windowHeight="20500" activeTab="1" xr2:uid="{779FA029-616C-294B-9FFE-D0BD9BFD1AEB}"/>
+    <workbookView xWindow="25120" yWindow="600" windowWidth="23500" windowHeight="20500" activeTab="1" xr2:uid="{779FA029-616C-294B-9FFE-D0BD9BFD1AEB}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -249,9 +249,6 @@
     <t xml:space="preserve">GET </t>
   </si>
   <si>
-    <t>my/flashcard:id/edit</t>
-  </si>
-  <si>
     <t>my/play</t>
   </si>
   <si>
@@ -373,6 +370,9 @@
   </si>
   <si>
     <t>api/my/collections/:id/flashcards/:id</t>
+  </si>
+  <si>
+    <t>my/flashcard/:id/edit</t>
   </si>
 </sst>
 </file>
@@ -837,7 +837,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="3" t="b">
         <v>0</v>
@@ -869,7 +869,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>16</v>
@@ -895,7 +895,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>17</v>
@@ -924,7 +924,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G7" s="7">
         <v>401</v>
@@ -944,13 +944,13 @@
         <v>23</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -982,7 +982,7 @@
         <v>26</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1010,7 +1010,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" s="3" t="b">
         <v>1</v>
@@ -1030,13 +1030,13 @@
         <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="C13" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>25</v>
@@ -1053,7 +1053,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="3" t="b">
         <v>1</v>
@@ -1082,7 +1082,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="3" t="b">
         <v>1</v>
@@ -1105,13 +1105,13 @@
         <v>18</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>34</v>
@@ -1125,13 +1125,13 @@
         <v>20</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>32</v>
@@ -1148,7 +1148,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" s="3" t="b">
         <v>1</v>
@@ -1200,7 +1200,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" s="3" t="b">
         <v>1</v>
@@ -1209,7 +1209,7 @@
         <v>53</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>31</v>
@@ -1228,7 +1228,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1359,10 +1359,10 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1370,16 +1370,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1387,16 +1387,16 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1411,16 +1411,16 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1428,16 +1428,16 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
         <v>66</v>
       </c>
-      <c r="C14" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>67</v>
-      </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1445,16 +1445,16 @@
         <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1469,16 +1469,16 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1486,16 +1486,16 @@
         <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added authentication API, adjusted database schema
</commit_message>
<xml_diff>
--- a/resources/API docs.xlsx
+++ b/resources/API docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arturaronov/Desktop/Programming/fswdi/unit-2/unit-2-project/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE2AFD6-C572-434B-8F1C-10E5F13079FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94B4971-64D5-5F43-A70C-F8AFFD026385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25120" yWindow="600" windowWidth="23500" windowHeight="20500" activeTab="1" xr2:uid="{779FA029-616C-294B-9FFE-D0BD9BFD1AEB}"/>
+    <workbookView xWindow="27060" yWindow="500" windowWidth="24100" windowHeight="20500" xr2:uid="{779FA029-616C-294B-9FFE-D0BD9BFD1AEB}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="95">
   <si>
     <t>API</t>
   </si>
@@ -136,9 +136,6 @@
 dateCreated,
 dateEdited,
 flashcards</t>
-  </si>
-  <si>
-    <t>src/controllers/api/my/collections/index.js</t>
   </si>
   <si>
     <t>api/my/collections</t>
@@ -315,9 +312,6 @@
     <t>src/views/my/collections/play.ejs</t>
   </si>
   <si>
-    <t>src/controllers/api/my/flashcards/index.js</t>
-  </si>
-  <si>
     <t>email,
 password</t>
   </si>
@@ -373,6 +367,9 @@
   </si>
   <si>
     <t>my/flashcard/:id/edit</t>
+  </si>
+  <si>
+    <t>src/controllers/api/my/flashcards/show.js</t>
   </si>
 </sst>
 </file>
@@ -782,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADFA567-0D34-C947-ABE1-1904C5F5623A}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -837,7 +834,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C3" s="3" t="b">
         <v>0</v>
@@ -869,7 +866,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>16</v>
@@ -895,7 +892,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>17</v>
@@ -924,7 +921,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G7" s="7">
         <v>401</v>
@@ -944,13 +941,13 @@
         <v>23</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -967,7 +964,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3" t="b">
         <v>1</v>
@@ -982,7 +979,7 @@
         <v>26</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -990,13 +987,13 @@
         <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>27</v>
@@ -1010,19 +1007,19 @@
         <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C12" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>26</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -1030,13 +1027,13 @@
         <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C13" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>25</v>
@@ -1045,7 +1042,7 @@
         <v>26</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -1053,19 +1050,19 @@
         <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C14" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>26</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1082,19 +1079,19 @@
         <v>8</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C16" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="G16" s="7">
         <v>406</v>
@@ -1105,16 +1102,16 @@
         <v>18</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C17" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G17" s="7">
         <v>401</v>
@@ -1125,22 +1122,22 @@
         <v>20</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C18" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="G18" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="153" x14ac:dyDescent="0.2">
@@ -1148,19 +1145,19 @@
         <v>9</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C19" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1177,22 +1174,22 @@
         <v>8</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1200,19 +1197,19 @@
         <v>18</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C22" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1227,7 +1224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C72B2D-D8D1-4E47-AB6F-A25D502EAF91}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1242,7 +1239,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -1263,7 +1260,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1271,16 +1268,16 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1288,16 +1285,16 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1312,16 +1309,16 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1329,16 +1326,16 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1353,16 +1350,16 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1370,16 +1367,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1387,16 +1384,16 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1411,16 +1408,16 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1428,33 +1425,33 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
         <v>65</v>
       </c>
-      <c r="C14" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>66</v>
-      </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1469,33 +1466,33 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up Controllers and Views to follow the Show / Create / Update /Delete naming convention
</commit_message>
<xml_diff>
--- a/resources/API docs.xlsx
+++ b/resources/API docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arturaronov/Desktop/Programming/fswdi/unit-2/unit-2-project/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94B4971-64D5-5F43-A70C-F8AFFD026385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02133E7D-91CB-6A48-B7CB-1CAD8FD2AF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27060" yWindow="500" windowWidth="24100" windowHeight="20500" xr2:uid="{779FA029-616C-294B-9FFE-D0BD9BFD1AEB}"/>
+    <workbookView xWindow="16020" yWindow="500" windowWidth="24100" windowHeight="20500" xr2:uid="{779FA029-616C-294B-9FFE-D0BD9BFD1AEB}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="92">
   <si>
     <t>API</t>
   </si>
@@ -108,13 +108,7 @@
     <t>PUT</t>
   </si>
   <si>
-    <t>api/my/profile/edit</t>
-  </si>
-  <si>
     <t>src/controllers/api/my/profile/show.js</t>
-  </si>
-  <si>
-    <t>src/controllers/api/my/profile/edit.js</t>
   </si>
   <si>
     <t>src/controllers/api/my/collections/create.js</t>
@@ -225,12 +219,6 @@
     <t>src/views/my/profile/edit.ejs</t>
   </si>
   <si>
-    <t>api/my/play</t>
-  </si>
-  <si>
-    <t>src/controllers/api/my/play.js</t>
-  </si>
-  <si>
     <t>src/controllers/api/my/collections/play.js</t>
   </si>
   <si>
@@ -246,67 +234,16 @@
     <t xml:space="preserve">GET </t>
   </si>
   <si>
-    <t>my/play</t>
-  </si>
-  <si>
-    <t>my/collection:id/play</t>
-  </si>
-  <si>
-    <t>src/controllers/pages/my/collections/new.js</t>
-  </si>
-  <si>
-    <t>my/collections/new</t>
-  </si>
-  <si>
-    <t>my/collections/:id/edit</t>
-  </si>
-  <si>
     <t>my/collections/:id/flashcards</t>
   </si>
   <si>
-    <t>my/collections/:id/new</t>
-  </si>
-  <si>
     <t>src/controllers/pages/my/flashcards/new.js</t>
   </si>
   <si>
-    <t>src/controllers/pages/my/flashcards/edit.js</t>
-  </si>
-  <si>
-    <t>src/controllers/pages/my/collections/edit.js</t>
-  </si>
-  <si>
-    <t>src/controllers/pages/my/play.js</t>
-  </si>
-  <si>
     <t>src/controllers/pages/my/collections/play.js</t>
   </si>
   <si>
-    <t>src/views/my/collections/index.ejs</t>
-  </si>
-  <si>
-    <t>src/controllers/pages/my/collections/index.js</t>
-  </si>
-  <si>
-    <t>src/views/my/collections/new.ejs</t>
-  </si>
-  <si>
-    <t>src/views/my/collections/edit.ejs</t>
-  </si>
-  <si>
-    <t>src/views/my/flashcards/index.ejs</t>
-  </si>
-  <si>
-    <t>src/controllers/pages/my/flashcards/index.js</t>
-  </si>
-  <si>
     <t>src/views/my/flashcards/new.ejs</t>
-  </si>
-  <si>
-    <t>src/views/my/flashcards/edit.ejs</t>
-  </si>
-  <si>
-    <t>src/views/my/play.ejs</t>
   </si>
   <si>
     <t>src/views/my/collections/play.ejs</t>
@@ -352,24 +289,73 @@
     <t>api/my/collections/:id/flashcards</t>
   </si>
   <si>
-    <t>api/my/collection/:id/play</t>
-  </si>
-  <si>
-    <t>Array of:
-id,
-name,
-dateCreated,
-dateEdited,
-flashcards</t>
-  </si>
-  <si>
-    <t>api/my/collections/:id/flashcards/:id</t>
-  </si>
-  <si>
-    <t>my/flashcard/:id/edit</t>
-  </si>
-  <si>
     <t>src/controllers/api/my/flashcards/show.js</t>
+  </si>
+  <si>
+    <t>api/my/play/:id</t>
+  </si>
+  <si>
+    <t>/api/collections/:collectionId/flashcards/:flashcardId</t>
+  </si>
+  <si>
+    <t>api/my/profile/update</t>
+  </si>
+  <si>
+    <t>src/controllers/api/my/profile/update.js</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>src/controllers/pages/show.js</t>
+  </si>
+  <si>
+    <t>src/views/show.ejs</t>
+  </si>
+  <si>
+    <t>src/controllers/pages/my/collections/update.js</t>
+  </si>
+  <si>
+    <t>src/views/my/collections/update.ejs</t>
+  </si>
+  <si>
+    <t>my/collections/:id/update</t>
+  </si>
+  <si>
+    <t>src/controllers/pages/my/collections/create.js</t>
+  </si>
+  <si>
+    <t>my/collections/create</t>
+  </si>
+  <si>
+    <t>src/views/my/collections/create.ejs</t>
+  </si>
+  <si>
+    <t>src/views/my/collections/show.ejs</t>
+  </si>
+  <si>
+    <t>src/controllers/pages/my/collections/show.js</t>
+  </si>
+  <si>
+    <t>src/controllers/pages/my/flashcards/show.js</t>
+  </si>
+  <si>
+    <t>my/collections/:id/show</t>
+  </si>
+  <si>
+    <t>src/views/my/flashcards/update.ejs</t>
+  </si>
+  <si>
+    <t>/my/collections/:id/flashcards/:id</t>
+  </si>
+  <si>
+    <t>src/controllers/pages/my/flashcards/update.js</t>
+  </si>
+  <si>
+    <t>/my/collection/:id/play</t>
+  </si>
+  <si>
+    <t>src/views/my/flashcards/show.ejs</t>
   </si>
 </sst>
 </file>
@@ -427,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -463,6 +449,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,16 +764,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADFA567-0D34-C947-ABE1-1904C5F5623A}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="3"/>
-    <col min="2" max="2" width="33.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="45" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="3"/>
     <col min="4" max="4" width="37.83203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="23.1640625" style="3" customWidth="1"/>
@@ -834,7 +821,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C3" s="3" t="b">
         <v>0</v>
@@ -866,7 +853,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>16</v>
@@ -892,7 +879,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>17</v>
@@ -918,10 +905,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="G7" s="7">
         <v>401</v>
@@ -931,23 +918,23 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>21</v>
+      <c r="B8" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="C8" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>23</v>
+      <c r="D8" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -964,22 +951,22 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="G10" s="7" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -987,16 +974,16 @@
         <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G11" s="7">
         <v>401</v>
@@ -1004,212 +991,172 @@
     </row>
     <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C12" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>29</v>
+      <c r="D12" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C13" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="G15" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="B17" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="7">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="7">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="170" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="7">
+      <c r="G18" s="7">
         <v>401</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C18" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G19" s="7" t="s">
+      <c r="B20" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C22" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>30</v>
+      <c r="G20" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1225,7 +1172,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1239,7 +1186,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -1260,7 +1207,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1268,16 +1215,16 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1285,214 +1232,214 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
       <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
         <v>42</v>
       </c>
-      <c r="E4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" t="s">
-        <v>49</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E8" t="s">
         <v>48</v>
       </c>
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" t="s">
-        <v>70</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" t="s">
-        <v>72</v>
+      <c r="B10" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" t="s">
-        <v>73</v>
+      <c r="B11" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>75</v>
-      </c>
-      <c r="E13" t="s">
-        <v>74</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" t="s">
-        <v>76</v>
+      <c r="B14" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B15" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" t="s">
-        <v>78</v>
-      </c>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>